<commit_message>
Tested Random Forest and running model on all datapoints
</commit_message>
<xml_diff>
--- a/gradCam/YoloVGGBaseModelAvgConvTrials.xlsx
+++ b/gradCam/YoloVGGBaseModelAvgConvTrials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josem\Documents\schoolWork\MQP\Git\Brain-Scans-MQP\gradCam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040CA40F-19CC-4DBC-B9DA-E51A00C2F3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B897107D-6918-4766-BB60-21675BC8C505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="450" windowWidth="28800" windowHeight="15375" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="23250" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trainMSE" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,7 +72,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFD4D4D4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -97,17 +102,103 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -386,19 +477,20 @@
   <dimension ref="A3:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -493,7 +585,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>50.804051325871299</v>
       </c>
       <c r="C4">
@@ -561,7 +653,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>2.0241793634799801</v>
       </c>
       <c r="C5">
@@ -629,7 +721,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>1.9790952492218701</v>
       </c>
       <c r="C6">
@@ -724,7 +816,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>1.9317812690367999</v>
       </c>
       <c r="C7">
@@ -819,15 +911,211 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3">
+        <v>1.8612152796525201</v>
+      </c>
+      <c r="C8">
+        <v>0.84477911201807099</v>
+      </c>
+      <c r="D8">
+        <v>0.51097196799058098</v>
+      </c>
+      <c r="E8">
+        <v>0.42541528607790202</v>
+      </c>
+      <c r="F8">
+        <v>0.35822879179165901</v>
+      </c>
+      <c r="G8">
+        <v>0.36296081485656501</v>
+      </c>
+      <c r="H8">
+        <v>0.32630943908141202</v>
+      </c>
+      <c r="I8">
+        <v>0.50573689375932396</v>
+      </c>
+      <c r="J8">
+        <v>0.355900055513932</v>
+      </c>
+      <c r="K8">
+        <v>0.28035792937645498</v>
+      </c>
+      <c r="L8">
+        <v>0.20401049118775499</v>
+      </c>
+      <c r="M8">
+        <v>0.20229306587806101</v>
+      </c>
+      <c r="N8">
+        <v>0.19331612609899901</v>
+      </c>
+      <c r="O8">
+        <v>0.18857670976565399</v>
+      </c>
+      <c r="P8">
+        <v>0.19279269702159399</v>
+      </c>
+      <c r="Q8">
+        <v>0.18670854717492999</v>
+      </c>
+      <c r="R8">
+        <v>0.20091318052548601</v>
+      </c>
+      <c r="S8">
+        <v>0.185326438683729</v>
+      </c>
+      <c r="T8">
+        <v>0.19729521182867099</v>
+      </c>
+      <c r="U8">
+        <v>0.18581424596217899</v>
+      </c>
+      <c r="V8">
+        <v>0.18313351330848801</v>
+      </c>
+      <c r="W8">
+        <v>0.18237668275833099</v>
+      </c>
+      <c r="X8">
+        <v>0.18006151054914099</v>
+      </c>
+      <c r="Y8">
+        <v>0.18682098331359701</v>
+      </c>
+      <c r="Z8">
+        <v>0.17925884574651699</v>
+      </c>
+      <c r="AA8">
+        <v>0.18181073665618799</v>
+      </c>
+      <c r="AB8">
+        <v>0.17705390888910999</v>
+      </c>
+      <c r="AC8">
+        <v>0.17985165577668399</v>
+      </c>
+      <c r="AD8">
+        <v>0.18559324855987799</v>
+      </c>
+      <c r="AE8">
+        <v>0.18877861763422299</v>
+      </c>
     </row>
     <row r="9" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3">
+        <v>2.0483712106943099</v>
+      </c>
+      <c r="C9">
+        <v>0.91975758224725701</v>
+      </c>
+      <c r="D9">
+        <v>0.47273546113417603</v>
+      </c>
+      <c r="E9">
+        <v>0.37175592894737503</v>
+      </c>
+      <c r="F9">
+        <v>0.37390006562838102</v>
+      </c>
+      <c r="G9">
+        <v>0.440360142061343</v>
+      </c>
+      <c r="H9">
+        <v>0.47728814757787202</v>
+      </c>
+      <c r="I9">
+        <v>0.31732447101519601</v>
+      </c>
+      <c r="J9">
+        <v>0.25272658524604902</v>
+      </c>
+      <c r="K9">
+        <v>0.24411510332272601</v>
+      </c>
+      <c r="L9">
+        <v>0.208647150259751</v>
+      </c>
+      <c r="M9">
+        <v>0.19384062060943</v>
+      </c>
+      <c r="N9">
+        <v>0.19892447155255499</v>
+      </c>
+      <c r="O9">
+        <v>0.19634744295707099</v>
+      </c>
+      <c r="P9">
+        <v>0.19150677495277801</v>
+      </c>
+      <c r="Q9">
+        <v>0.18594022267139801</v>
+      </c>
+      <c r="R9">
+        <v>0.18516861475431001</v>
+      </c>
+      <c r="S9">
+        <v>0.18855409553417701</v>
+      </c>
+      <c r="T9">
+        <v>0.19343304404845599</v>
+      </c>
+      <c r="U9">
+        <v>0.189103262355694</v>
+      </c>
+      <c r="V9">
+        <v>0.191503265729317</v>
+      </c>
+      <c r="W9">
+        <v>0.18291986103241201</v>
+      </c>
+      <c r="X9">
+        <v>0.17720358704145101</v>
+      </c>
+      <c r="Y9">
+        <v>0.184351757168769</v>
+      </c>
+      <c r="Z9">
+        <v>0.17898574929970901</v>
+      </c>
+      <c r="AA9">
+        <v>0.17704543356711999</v>
+      </c>
+      <c r="AB9">
+        <v>0.17946415337232399</v>
+      </c>
+      <c r="AC9">
+        <v>0.19092560043701701</v>
+      </c>
+      <c r="AD9">
+        <v>0.18358411238743699</v>
+      </c>
+      <c r="AE9">
+        <v>0.181899090225879</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B4:AE4">
+    <cfRule type="top10" dxfId="5" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:AE5">
+    <cfRule type="top10" dxfId="4" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:AE6">
+    <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:AE7">
+    <cfRule type="top10" dxfId="2" priority="4" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:AE8">
+    <cfRule type="top10" dxfId="1" priority="5" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:AE9">
+    <cfRule type="top10" dxfId="0" priority="6" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -837,20 +1125,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737BF290-449F-4E4D-8496-553CE1679F93}">
   <dimension ref="A3:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -945,7 +1234,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>50.804051325871299</v>
       </c>
       <c r="C4">
@@ -1013,7 +1302,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>1.8418010075886999</v>
       </c>
       <c r="C5">
@@ -1081,7 +1370,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>0.60191644231478303</v>
       </c>
       <c r="C6">
@@ -1176,7 +1465,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>0.86181932687759399</v>
       </c>
       <c r="C7">
@@ -1271,15 +1560,213 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3">
+        <v>0.65382417043050101</v>
+      </c>
+      <c r="C8">
+        <v>0.43709224959214499</v>
+      </c>
+      <c r="D8">
+        <v>0.40347446004549598</v>
+      </c>
+      <c r="E8">
+        <v>0.37161883215109498</v>
+      </c>
+      <c r="F8">
+        <v>0.34597503145535702</v>
+      </c>
+      <c r="G8">
+        <v>0.51445565621058098</v>
+      </c>
+      <c r="H8">
+        <v>0.37625828385353</v>
+      </c>
+      <c r="I8">
+        <v>0.44867259263992298</v>
+      </c>
+      <c r="J8">
+        <v>0.314673895637194</v>
+      </c>
+      <c r="K8">
+        <v>0.22719916204611401</v>
+      </c>
+      <c r="L8">
+        <v>0.21612749497095701</v>
+      </c>
+      <c r="M8">
+        <v>0.20366744200388501</v>
+      </c>
+      <c r="N8">
+        <v>0.17874434093634201</v>
+      </c>
+      <c r="O8">
+        <v>0.18161167204379999</v>
+      </c>
+      <c r="P8">
+        <v>0.170449544986089</v>
+      </c>
+      <c r="Q8">
+        <v>0.18710262576738901</v>
+      </c>
+      <c r="R8">
+        <v>0.17368193467458001</v>
+      </c>
+      <c r="S8">
+        <v>0.180419380466143</v>
+      </c>
+      <c r="T8">
+        <v>0.18210852146148601</v>
+      </c>
+      <c r="U8">
+        <v>0.173277333378791</v>
+      </c>
+      <c r="V8">
+        <v>0.168975740671157</v>
+      </c>
+      <c r="W8">
+        <v>0.17931834856669099</v>
+      </c>
+      <c r="X8">
+        <v>0.17644685010115299</v>
+      </c>
+      <c r="Y8">
+        <v>0.20787205298741601</v>
+      </c>
+      <c r="Z8">
+        <v>0.186538184682528</v>
+      </c>
+      <c r="AA8">
+        <v>0.195243924856185</v>
+      </c>
+      <c r="AB8">
+        <v>0.19813829660415599</v>
+      </c>
+      <c r="AC8">
+        <v>0.17795215050379401</v>
+      </c>
+      <c r="AD8">
+        <v>0.20204702019691401</v>
+      </c>
+      <c r="AE8">
+        <v>0.18370625376701299</v>
+      </c>
     </row>
     <row r="9" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3">
+        <v>1.2011740406354201</v>
+      </c>
+      <c r="C9">
+        <v>1.01620615522066</v>
+      </c>
+      <c r="D9">
+        <v>0.29462776581446298</v>
+      </c>
+      <c r="E9">
+        <v>0.33415421843528698</v>
+      </c>
+      <c r="F9">
+        <v>0.72466020782788598</v>
+      </c>
+      <c r="G9">
+        <v>0.37865042686462402</v>
+      </c>
+      <c r="H9">
+        <v>0.23407530287901501</v>
+      </c>
+      <c r="I9">
+        <v>0.23515600959459901</v>
+      </c>
+      <c r="J9">
+        <v>0.196558788418769</v>
+      </c>
+      <c r="K9">
+        <v>0.21600799759229</v>
+      </c>
+      <c r="L9">
+        <v>0.18439856668313301</v>
+      </c>
+      <c r="M9">
+        <v>0.184813405076662</v>
+      </c>
+      <c r="N9">
+        <v>0.18414380153020199</v>
+      </c>
+      <c r="O9">
+        <v>0.16664844751357999</v>
+      </c>
+      <c r="P9">
+        <v>0.173489689826965</v>
+      </c>
+      <c r="Q9">
+        <v>0.167944446206092</v>
+      </c>
+      <c r="R9">
+        <v>0.17592479785283399</v>
+      </c>
+      <c r="S9">
+        <v>0.19181536634763</v>
+      </c>
+      <c r="T9">
+        <v>0.169645031293233</v>
+      </c>
+      <c r="U9">
+        <v>0.17448720335960299</v>
+      </c>
+      <c r="V9">
+        <v>0.17761973539988199</v>
+      </c>
+      <c r="W9">
+        <v>0.17066912353038699</v>
+      </c>
+      <c r="X9">
+        <v>0.16919158895810399</v>
+      </c>
+      <c r="Y9">
+        <v>0.16505253811677201</v>
+      </c>
+      <c r="Z9">
+        <v>0.16798328856627101</v>
+      </c>
+      <c r="AA9">
+        <v>0.16412061452865601</v>
+      </c>
+      <c r="AB9">
+        <v>0.17359388868014</v>
+      </c>
+      <c r="AC9">
+        <v>0.161912937959035</v>
+      </c>
+      <c r="AD9">
+        <v>0.18553897738456701</v>
+      </c>
+      <c r="AE9">
+        <v>0.16924741864204401</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B5:V5">
+    <cfRule type="top10" dxfId="11" priority="6" bottom="1" rank="1"/>
+    <cfRule type="top10" priority="7" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:AE4">
+    <cfRule type="top10" dxfId="10" priority="8" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:AE6">
+    <cfRule type="top10" dxfId="9" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:AE7">
+    <cfRule type="top10" dxfId="8" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:AE8">
+    <cfRule type="top10" dxfId="7" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:AE9">
+    <cfRule type="top10" dxfId="6" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1289,19 +1776,20 @@
   <dimension ref="A3:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -1396,7 +1884,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>50.804051325871299</v>
       </c>
       <c r="C4">
@@ -1464,7 +1952,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>-2.3381899396920298</v>
       </c>
       <c r="C5">
@@ -1532,7 +2020,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>-2.9851975559391701</v>
       </c>
       <c r="C6">
@@ -1627,7 +2115,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>-2.4144758316078101</v>
       </c>
       <c r="C7">
@@ -1722,13 +2210,191 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3">
+        <v>-2.0281836890184399</v>
+      </c>
+      <c r="C8">
+        <v>-3.3302561500304999</v>
+      </c>
+      <c r="D8">
+        <v>-4.9714952259351701</v>
+      </c>
+      <c r="E8">
+        <v>-5.1550085159455801</v>
+      </c>
+      <c r="F8">
+        <v>-5.8306787839748404</v>
+      </c>
+      <c r="G8">
+        <v>-11.379355543909099</v>
+      </c>
+      <c r="H8">
+        <v>-8.2442458416948607</v>
+      </c>
+      <c r="I8">
+        <v>-10.2294123113493</v>
+      </c>
+      <c r="J8">
+        <v>-12.613000897301401</v>
+      </c>
+      <c r="K8">
+        <v>-10.2398612380609</v>
+      </c>
+      <c r="L8">
+        <v>-16.968979298145499</v>
+      </c>
+      <c r="M8">
+        <v>-17.1833124510486</v>
+      </c>
+      <c r="N8">
+        <v>-23.762466710602499</v>
+      </c>
+      <c r="O8">
+        <v>-19.900976872497001</v>
+      </c>
+      <c r="P8">
+        <v>-17.302843053173799</v>
+      </c>
+      <c r="Q8">
+        <v>-22.5240420464003</v>
+      </c>
+      <c r="R8">
+        <v>-17.488367576973001</v>
+      </c>
+      <c r="S8">
+        <v>-19.224931375123401</v>
+      </c>
+      <c r="T8">
+        <v>-19.696978095475998</v>
+      </c>
+      <c r="U8">
+        <v>-20.288651249502099</v>
+      </c>
+      <c r="V8">
+        <v>-20.419459328473199</v>
+      </c>
+      <c r="W8">
+        <v>-23.960266101544899</v>
+      </c>
+      <c r="X8">
+        <v>-21.589928117452502</v>
+      </c>
+      <c r="Y8">
+        <v>-24.2408015420712</v>
+      </c>
+      <c r="Z8">
+        <v>-24.517069744080199</v>
+      </c>
+      <c r="AA8">
+        <v>-19.178329893106898</v>
+      </c>
+      <c r="AB8">
+        <v>-25.731470819682301</v>
+      </c>
+      <c r="AC8">
+        <v>-20.768541947356599</v>
+      </c>
+      <c r="AD8">
+        <v>-18.066524179391301</v>
+      </c>
+      <c r="AE8">
+        <v>-21.022397626282199</v>
+      </c>
     </row>
     <row r="9" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3">
+        <v>-2.1026392037585402</v>
+      </c>
+      <c r="C9">
+        <v>-3.5221534499349798</v>
+      </c>
+      <c r="D9">
+        <v>-6.0465413035341404</v>
+      </c>
+      <c r="E9">
+        <v>-5.0930671940596799</v>
+      </c>
+      <c r="F9">
+        <v>-6.4654865579637297</v>
+      </c>
+      <c r="G9">
+        <v>-9.1642909339570693</v>
+      </c>
+      <c r="H9">
+        <v>-7.6355911930809199</v>
+      </c>
+      <c r="I9">
+        <v>-9.1460187897948995</v>
+      </c>
+      <c r="J9">
+        <v>-10.6262394784561</v>
+      </c>
+      <c r="K9">
+        <v>-12.5843668919604</v>
+      </c>
+      <c r="L9">
+        <v>-18.3141285395232</v>
+      </c>
+      <c r="M9">
+        <v>-18.200487090605002</v>
+      </c>
+      <c r="N9">
+        <v>-20.079927314454999</v>
+      </c>
+      <c r="O9">
+        <v>-17.3483624317962</v>
+      </c>
+      <c r="P9">
+        <v>-20.814548599024501</v>
+      </c>
+      <c r="Q9">
+        <v>-19.4246796895406</v>
+      </c>
+      <c r="R9">
+        <v>-19.773796067915001</v>
+      </c>
+      <c r="S9">
+        <v>-24.486112653937099</v>
+      </c>
+      <c r="T9">
+        <v>-17.241480898765801</v>
+      </c>
+      <c r="U9">
+        <v>-19.793245446231602</v>
+      </c>
+      <c r="V9">
+        <v>-19.148106090493201</v>
+      </c>
+      <c r="W9">
+        <v>-28.925403140653899</v>
+      </c>
+      <c r="X9">
+        <v>-23.337319834366301</v>
+      </c>
+      <c r="Y9">
+        <v>-20.973911189728401</v>
+      </c>
+      <c r="Z9">
+        <v>-24.475902267378601</v>
+      </c>
+      <c r="AA9">
+        <v>-21.874778907129102</v>
+      </c>
+      <c r="AB9">
+        <v>-32.033955607207098</v>
+      </c>
+      <c r="AC9">
+        <v>-19.028683115827398</v>
+      </c>
+      <c r="AD9">
+        <v>-19.109807597218101</v>
+      </c>
+      <c r="AE9">
+        <v>-26.587402595660901</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1739,20 +2405,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA94F6-29BF-4BF1-AC46-195D676E254A}">
   <dimension ref="A3:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -1847,7 +2514,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>50.804051325871299</v>
       </c>
       <c r="C4">
@@ -1915,7 +2582,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>-2.9178632780246598</v>
       </c>
       <c r="C5">
@@ -1983,7 +2650,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>-5.6125960598949103</v>
       </c>
       <c r="C6">
@@ -2078,7 +2745,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>-2.54358317743305</v>
       </c>
       <c r="C7">
@@ -2173,13 +2840,191 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3">
+        <v>-2.4029522613446899</v>
+      </c>
+      <c r="C8">
+        <v>-6.5252679792847701</v>
+      </c>
+      <c r="D8">
+        <v>-4.7318448857497497</v>
+      </c>
+      <c r="E8">
+        <v>-7.5968659074334202</v>
+      </c>
+      <c r="F8">
+        <v>-12.695907936532301</v>
+      </c>
+      <c r="G8">
+        <v>-4.7316095921733403</v>
+      </c>
+      <c r="H8">
+        <v>-8.1126076107351892</v>
+      </c>
+      <c r="I8">
+        <v>-12.0265105245604</v>
+      </c>
+      <c r="J8">
+        <v>-5.6911987249210796</v>
+      </c>
+      <c r="K8">
+        <v>-10.833796485263001</v>
+      </c>
+      <c r="L8">
+        <v>-10.293715584294899</v>
+      </c>
+      <c r="M8">
+        <v>-10.009057414525</v>
+      </c>
+      <c r="N8">
+        <v>-18.674767238692599</v>
+      </c>
+      <c r="O8">
+        <v>-24.3803586120769</v>
+      </c>
+      <c r="P8">
+        <v>-26.150300369512301</v>
+      </c>
+      <c r="Q8">
+        <v>-11.473805635693299</v>
+      </c>
+      <c r="R8">
+        <v>-26.290799829953599</v>
+      </c>
+      <c r="S8">
+        <v>-33.972118720283298</v>
+      </c>
+      <c r="T8">
+        <v>-27.325666981951599</v>
+      </c>
+      <c r="U8">
+        <v>-25.856426737236799</v>
+      </c>
+      <c r="V8">
+        <v>-33.788338625940703</v>
+      </c>
+      <c r="W8">
+        <v>-15.322050113620801</v>
+      </c>
+      <c r="X8">
+        <v>-49.037805657812598</v>
+      </c>
+      <c r="Y8">
+        <v>-16.397551157495599</v>
+      </c>
+      <c r="Z8">
+        <v>-22.430657751390498</v>
+      </c>
+      <c r="AA8">
+        <v>-15.7983733569845</v>
+      </c>
+      <c r="AB8">
+        <v>-10.823148345111999</v>
+      </c>
+      <c r="AC8">
+        <v>-22.8534046848259</v>
+      </c>
+      <c r="AD8">
+        <v>-15.371627210016999</v>
+      </c>
+      <c r="AE8">
+        <v>-22.5009904136665</v>
+      </c>
     </row>
     <row r="9" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3">
+        <v>-3.2546749815824998</v>
+      </c>
+      <c r="C9">
+        <v>-3.2396034049147802</v>
+      </c>
+      <c r="D9">
+        <v>-6.6889469864088502</v>
+      </c>
+      <c r="E9">
+        <v>-26.442800153243699</v>
+      </c>
+      <c r="F9">
+        <v>-5.8462950979985404</v>
+      </c>
+      <c r="G9">
+        <v>-9.1914077179037896</v>
+      </c>
+      <c r="H9">
+        <v>-11.390540595151</v>
+      </c>
+      <c r="I9">
+        <v>-11.7609023688482</v>
+      </c>
+      <c r="J9">
+        <v>-18.683860257186002</v>
+      </c>
+      <c r="K9">
+        <v>-12.593600683765199</v>
+      </c>
+      <c r="L9">
+        <v>-25.964924826601699</v>
+      </c>
+      <c r="M9">
+        <v>-22.893146683571398</v>
+      </c>
+      <c r="N9">
+        <v>-27.425293863236998</v>
+      </c>
+      <c r="O9">
+        <v>-29.190764856569999</v>
+      </c>
+      <c r="P9">
+        <v>-27.859590339204001</v>
+      </c>
+      <c r="Q9">
+        <v>-37.279043574158102</v>
+      </c>
+      <c r="R9">
+        <v>-24.1397113215682</v>
+      </c>
+      <c r="S9">
+        <v>-13.3658073425868</v>
+      </c>
+      <c r="T9">
+        <v>-27.915574345191999</v>
+      </c>
+      <c r="U9">
+        <v>-18.212944085803201</v>
+      </c>
+      <c r="V9">
+        <v>-21.160313900592499</v>
+      </c>
+      <c r="W9">
+        <v>-30.929619528927901</v>
+      </c>
+      <c r="X9">
+        <v>-25.293498247817698</v>
+      </c>
+      <c r="Y9">
+        <v>-39.073384963494</v>
+      </c>
+      <c r="Z9">
+        <v>-29.0115641643219</v>
+      </c>
+      <c r="AA9">
+        <v>-38.207251453636601</v>
+      </c>
+      <c r="AB9">
+        <v>-26.7525314591424</v>
+      </c>
+      <c r="AC9">
+        <v>-44.176320579423802</v>
+      </c>
+      <c r="AD9">
+        <v>-15.443101571737699</v>
+      </c>
+      <c r="AE9">
+        <v>-32.946464103258201</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>